<commit_message>
Change on whatsapp project
</commit_message>
<xml_diff>
--- a/SDET_Project_Group4_WhatsApp.xlsx
+++ b/SDET_Project_Group4_WhatsApp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://persistentsystems-my.sharepoint.com/personal/sanmati_porlekar_persistent_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simran_babasab\Desktop\Whatsapp\SDET_Group4_WhatsApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2006" documentId="8_{77F13E54-295A-4D80-B39D-CA8D588720A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD11C2D5-BAFB-44C8-89B9-C3BCF0E8569B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C40A628-1827-4AE4-8ABC-6C63997FBEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{02E32A95-A356-4AD4-AD14-246839B8DAD6}"/>
+    <workbookView xWindow="3980" yWindow="2810" windowWidth="14400" windowHeight="7270" firstSheet="1" activeTab="4" xr2:uid="{02E32A95-A356-4AD4-AD14-246839B8DAD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1523,9 +1522,6 @@
     <t>1. User must download the whatsapp 2.Internet must be ON.</t>
   </si>
   <si>
-    <t xml:space="preserve">User Registed </t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -1971,6 +1967,9 @@
   </si>
   <si>
     <t xml:space="preserve">1.Open  the app </t>
+  </si>
+  <si>
+    <t>User Registed .</t>
   </si>
 </sst>
 </file>
@@ -2472,21 +2471,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="68.7109375" customWidth="1"/>
-    <col min="2" max="2" width="86.85546875" customWidth="1"/>
+    <col min="1" max="1" width="68.7265625" customWidth="1"/>
+    <col min="2" max="2" width="86.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:2">
       <c r="A1" s="7"/>
     </row>
-    <row r="2" spans="1:2" ht="18.75">
+    <row r="2" spans="1:2" ht="18.5">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="21" customFormat="1" ht="15.75">
+    <row r="3" spans="1:2" s="21" customFormat="1" ht="15.5">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="60.75">
+    <row r="9" spans="1:2" ht="58">
       <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
@@ -2560,7 +2559,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15">
+    <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -2572,33 +2571,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E8F296-A316-47A4-B854-434EB02AC5A3}">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="D46" sqref="D46:D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" customWidth="1"/>
-    <col min="5" max="5" width="57.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="39.1796875" customWidth="1"/>
+    <col min="4" max="4" width="40.1796875" customWidth="1"/>
+    <col min="5" max="5" width="57.81640625" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" customWidth="1"/>
+    <col min="9" max="9" width="12.26953125" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:12">
       <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D1" s="17"/>
     </row>
-    <row r="3" spans="1:12" s="18" customFormat="1" ht="15">
+    <row r="3" spans="1:12" s="18" customFormat="1">
       <c r="A3" s="12" t="s">
         <v>21</v>
       </c>
@@ -2662,7 +2661,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15">
+    <row r="9" spans="1:12">
       <c r="C9" s="2" t="s">
         <v>39</v>
       </c>
@@ -2681,7 +2680,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15">
+    <row r="11" spans="1:12">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2694,10 +2693,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="15"/>
-    <row r="13" spans="1:12" ht="15"/>
-    <row r="14" spans="1:12" ht="15"/>
-    <row r="15" spans="1:12" ht="15">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2714,7 +2710,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15">
+    <row r="16" spans="1:12">
       <c r="D16" t="s">
         <v>49</v>
       </c>
@@ -2722,21 +2718,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5">
       <c r="E17" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5">
       <c r="E18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15"/>
-    <row r="20" spans="1:5" ht="15"/>
-    <row r="21" spans="1:5" ht="15"/>
-    <row r="22" spans="1:5" ht="15"/>
-    <row r="23" spans="1:5" ht="15">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2753,7 +2745,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15">
+    <row r="24" spans="1:5">
       <c r="D24" t="s">
         <v>58</v>
       </c>
@@ -2761,25 +2753,22 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15">
+    <row r="25" spans="1:5">
       <c r="E25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15">
+    <row r="26" spans="1:5">
       <c r="E26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15">
+    <row r="27" spans="1:5">
       <c r="E27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15"/>
-    <row r="29" spans="1:5" ht="15"/>
-    <row r="30" spans="1:5" ht="15"/>
-    <row r="31" spans="1:5" ht="15">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -2796,7 +2785,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15">
+    <row r="32" spans="1:5">
       <c r="D32" t="s">
         <v>58</v>
       </c>
@@ -2804,8 +2793,6 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15"/>
-    <row r="34" spans="1:5" ht="15"/>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>68</v>
@@ -2839,7 +2826,7 @@
     <row r="40" spans="1:5" ht="16.5">
       <c r="C40" s="6"/>
     </row>
-    <row r="41" spans="1:5" ht="15">
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -2881,7 +2868,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15">
+    <row r="47" spans="1:5">
       <c r="D47" t="s">
         <v>58</v>
       </c>
@@ -2895,9 +2882,6 @@
     <row r="49" spans="3:3" ht="16.5">
       <c r="C49" s="3"/>
     </row>
-    <row r="50" spans="3:3" ht="15"/>
-    <row r="51" spans="3:3" ht="15"/>
-    <row r="52" spans="3:3" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2911,22 +2895,22 @@
       <selection activeCell="L127" sqref="L127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="43.81640625" customWidth="1"/>
+    <col min="3" max="3" width="34.7265625" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
     <col min="6" max="6" width="42" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="28.54296875" customWidth="1"/>
+    <col min="9" max="9" width="30.26953125" customWidth="1"/>
+    <col min="10" max="10" width="17.453125" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" customWidth="1"/>
+    <col min="12" max="12" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="16" customFormat="1" ht="15">
+    <row r="1" spans="1:8" s="16" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>83</v>
       </c>
@@ -2952,7 +2936,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15">
+    <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
         <v>90</v>
       </c>
@@ -3043,7 +3027,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15">
+    <row r="9" spans="1:8">
       <c r="F9" s="2" t="s">
         <v>107</v>
       </c>
@@ -3228,7 +3212,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15">
+    <row r="26" spans="1:9">
       <c r="B26" t="s">
         <v>138</v>
       </c>
@@ -4310,15 +4294,15 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="18" customFormat="1">
@@ -5160,24 +5144,24 @@
   <dimension ref="A1:L159"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="37.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" customWidth="1"/>
+    <col min="3" max="3" width="36.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="37.1796875" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="16" customFormat="1" ht="15">
+    <row r="1" spans="1:12" s="16" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>83</v>
       </c>
@@ -5215,7 +5199,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30.75">
+    <row r="3" spans="1:12" ht="29">
       <c r="A3" s="5" t="s">
         <v>90</v>
       </c>
@@ -5241,16 +5225,16 @@
         <v>95</v>
       </c>
       <c r="I3" t="s">
+        <v>526</v>
+      </c>
+      <c r="J3" t="s">
         <v>377</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>378</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>379</v>
-      </c>
-      <c r="L3" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5261,16 +5245,15 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15"/>
-    <row r="7" spans="1:12" ht="91.5">
+    <row r="7" spans="1:12" ht="72.5">
       <c r="A7" t="s">
         <v>98</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>381</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>382</v>
       </c>
       <c r="D7" t="s">
         <v>93</v>
@@ -5285,16 +5268,16 @@
         <v>1000000000</v>
       </c>
       <c r="H7" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>384</v>
-      </c>
       <c r="J7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -5313,7 +5296,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15">
+    <row r="10" spans="1:12">
       <c r="F10" s="2" t="s">
         <v>107</v>
       </c>
@@ -5323,13 +5306,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15"/>
-    <row r="14" spans="1:12" ht="30.75">
+    <row r="14" spans="1:12" ht="29">
       <c r="A14" t="s">
         <v>111</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C14" t="s">
         <v>113</v>
@@ -5347,13 +5329,13 @@
         <v>115</v>
       </c>
       <c r="I14" t="s">
+        <v>385</v>
+      </c>
+      <c r="J14" t="s">
+        <v>377</v>
+      </c>
+      <c r="L14" t="s">
         <v>386</v>
-      </c>
-      <c r="J14" t="s">
-        <v>378</v>
-      </c>
-      <c r="L14" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -5378,7 +5360,6 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15"/>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>121</v>
@@ -5402,13 +5383,13 @@
         <v>124</v>
       </c>
       <c r="I19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L19" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -5425,7 +5406,7 @@
         <v>125</v>
       </c>
       <c r="I20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -5444,7 +5425,6 @@
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15"/>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>129</v>
@@ -5468,13 +5448,13 @@
         <v>131</v>
       </c>
       <c r="I25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L25" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -5491,7 +5471,7 @@
         <v>133</v>
       </c>
       <c r="I26" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -5502,13 +5482,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15"/>
-    <row r="30" spans="1:12" ht="45.75">
+    <row r="30" spans="1:12" ht="43.5">
       <c r="A30" t="s">
         <v>135</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C30" t="s">
         <v>113</v>
@@ -5526,16 +5505,16 @@
         <v>137</v>
       </c>
       <c r="I30" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L30" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="15">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="B31" t="s">
         <v>203</v>
       </c>
@@ -5574,12 +5553,12 @@
         <v>143</v>
       </c>
       <c r="I33" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="I34" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -5605,13 +5584,13 @@
         <v>146</v>
       </c>
       <c r="I36" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J36" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L36" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -5646,8 +5625,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15"/>
-    <row r="43" spans="1:12" ht="30.75">
+    <row r="43" spans="1:12" ht="29">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -5673,10 +5651,10 @@
         <v>154</v>
       </c>
       <c r="J43" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L43" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -5693,7 +5671,7 @@
         <v>156</v>
       </c>
       <c r="I44" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -5717,8 +5695,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15"/>
-    <row r="50" spans="1:12" ht="30.75">
+    <row r="50" spans="1:12" ht="29">
       <c r="A50" t="s">
         <v>161</v>
       </c>
@@ -5741,13 +5718,13 @@
         <v>163</v>
       </c>
       <c r="I50" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J50" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L50" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -5777,8 +5754,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15"/>
-    <row r="56" spans="1:12" ht="45.75">
+    <row r="56" spans="1:12" ht="43.5">
       <c r="A56" t="s">
         <v>167</v>
       </c>
@@ -5801,13 +5777,13 @@
         <v>169</v>
       </c>
       <c r="I56" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J56" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L56" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -5842,8 +5818,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15"/>
-    <row r="63" spans="1:12" ht="30.75">
+    <row r="63" spans="1:12" ht="29">
       <c r="A63" t="s">
         <v>175</v>
       </c>
@@ -5866,13 +5841,13 @@
         <v>177</v>
       </c>
       <c r="I63" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J63" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L63" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -5902,7 +5877,6 @@
         <v>181</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15"/>
     <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>182</v>
@@ -5926,13 +5900,13 @@
         <v>169</v>
       </c>
       <c r="I69" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J69" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L69" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -5962,7 +5936,6 @@
         <v>185</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15"/>
     <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>186</v>
@@ -5986,13 +5959,13 @@
         <v>188</v>
       </c>
       <c r="I75" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J75" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L75" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -6035,7 +6008,6 @@
         <v>193</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15"/>
     <row r="83" spans="1:12">
       <c r="A83" t="s">
         <v>194</v>
@@ -6062,10 +6034,10 @@
         <v>196</v>
       </c>
       <c r="J83" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L83" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -6082,7 +6054,7 @@
         <v>156</v>
       </c>
       <c r="I84" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -6106,7 +6078,6 @@
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15"/>
     <row r="90" spans="1:12">
       <c r="A90" t="s">
         <v>200</v>
@@ -6130,13 +6101,13 @@
         <v>202</v>
       </c>
       <c r="I90" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J90" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L90" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -6153,7 +6124,7 @@
         <v>205</v>
       </c>
       <c r="I91" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -6172,8 +6143,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15"/>
-    <row r="96" spans="1:12" ht="30.75">
+    <row r="96" spans="1:12" ht="29">
       <c r="A96" t="s">
         <v>209</v>
       </c>
@@ -6240,13 +6210,13 @@
         <v>216</v>
       </c>
       <c r="I102" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J102" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L102" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -6273,8 +6243,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15"/>
-    <row r="108" spans="1:12" ht="30.75">
+    <row r="108" spans="1:12" ht="29">
       <c r="A108" t="s">
         <v>220</v>
       </c>
@@ -6297,13 +6266,13 @@
         <v>222</v>
       </c>
       <c r="I108" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J108" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L108" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="109" spans="1:12">
@@ -6320,7 +6289,7 @@
         <v>224</v>
       </c>
       <c r="I109" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="110" spans="1:12">
@@ -6341,7 +6310,6 @@
         <v>227</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="15"/>
     <row r="115" spans="1:12">
       <c r="A115" t="s">
         <v>228</v>
@@ -6365,13 +6333,13 @@
         <v>230</v>
       </c>
       <c r="I115" t="s">
+        <v>406</v>
+      </c>
+      <c r="J115" t="s">
         <v>407</v>
       </c>
-      <c r="J115" t="s">
-        <v>408</v>
-      </c>
       <c r="L115" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="116" spans="1:12">
@@ -6388,7 +6356,7 @@
         <v>231</v>
       </c>
       <c r="I116" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -6407,8 +6375,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="15"/>
-    <row r="121" spans="1:12" ht="30.75">
+    <row r="121" spans="1:12" ht="29">
       <c r="A121" t="s">
         <v>234</v>
       </c>
@@ -6431,13 +6398,13 @@
         <v>237</v>
       </c>
       <c r="I121" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J121" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L121" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="122" spans="1:12">
@@ -6475,13 +6442,12 @@
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="15"/>
-    <row r="128" spans="1:12" ht="30.75">
+    <row r="128" spans="1:12" ht="29">
       <c r="A128" t="s">
         <v>243</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C128" t="s">
         <v>113</v>
@@ -6499,13 +6465,13 @@
         <v>245</v>
       </c>
       <c r="I128" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J128" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L128" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="129" spans="1:12">
@@ -6554,13 +6520,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="15"/>
-    <row r="136" spans="1:12" ht="30.75">
+    <row r="136" spans="1:12" ht="29">
       <c r="A136" t="s">
         <v>252</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C136" t="s">
         <v>113</v>
@@ -6578,13 +6543,13 @@
         <v>254</v>
       </c>
       <c r="I136" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J136" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L136" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="137" spans="1:12">
@@ -6645,13 +6610,12 @@
         <v>264</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="15"/>
-    <row r="147" spans="1:12" ht="45.75">
+    <row r="147" spans="1:12" ht="43.5">
       <c r="A147" t="s">
         <v>265</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C147" t="s">
         <v>113</v>
@@ -6669,13 +6633,13 @@
         <v>268</v>
       </c>
       <c r="I147" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J147" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L147" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="148" spans="1:12">
@@ -6692,7 +6656,7 @@
         <v>271</v>
       </c>
       <c r="I148" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="149" spans="1:12">
@@ -6745,7 +6709,6 @@
         <v>278</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="15"/>
     <row r="158" spans="1:12">
       <c r="A158" t="s">
         <v>279</v>
@@ -6769,13 +6732,13 @@
         <v>281</v>
       </c>
       <c r="I158" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J158" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L158" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="159" spans="1:12">
@@ -6805,22 +6768,22 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" s="13" customFormat="1">
       <c r="A2" s="13" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B3" t="s">
         <v>420</v>
-      </c>
-      <c r="B3" t="s">
-        <v>421</v>
       </c>
       <c r="C3" t="s">
         <v>292</v>
@@ -6836,73 +6799,73 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B5" t="s">
         <v>422</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>423</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>424</v>
-      </c>
-      <c r="D5" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>423</v>
+      </c>
+      <c r="B6" t="s">
+        <v>425</v>
+      </c>
+      <c r="C6" t="s">
+        <v>426</v>
+      </c>
+      <c r="D6" t="s">
         <v>424</v>
-      </c>
-      <c r="B6" t="s">
-        <v>426</v>
-      </c>
-      <c r="C6" t="s">
-        <v>427</v>
-      </c>
-      <c r="D6" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>426</v>
+      </c>
+      <c r="B7" t="s">
         <v>427</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>428</v>
       </c>
-      <c r="C7" t="s">
-        <v>429</v>
-      </c>
       <c r="D7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>428</v>
+      </c>
+      <c r="B8" t="s">
         <v>429</v>
-      </c>
-      <c r="B8" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="13" customFormat="1">
       <c r="A11" s="13" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>419</v>
+      </c>
+      <c r="B12" t="s">
         <v>420</v>
-      </c>
-      <c r="B12" t="s">
-        <v>421</v>
       </c>
       <c r="C12" t="s">
         <v>292</v>
@@ -6913,68 +6876,68 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B14" t="s">
+        <v>432</v>
+      </c>
+      <c r="C14" t="s">
+        <v>423</v>
+      </c>
+      <c r="D14" t="s">
         <v>433</v>
-      </c>
-      <c r="C14" t="s">
-        <v>424</v>
-      </c>
-      <c r="D14" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>423</v>
+      </c>
+      <c r="B15" t="s">
+        <v>434</v>
+      </c>
+      <c r="C15" t="s">
+        <v>426</v>
+      </c>
+      <c r="D15" t="s">
         <v>424</v>
-      </c>
-      <c r="B15" t="s">
-        <v>435</v>
-      </c>
-      <c r="C15" t="s">
-        <v>427</v>
-      </c>
-      <c r="D15" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D16" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B17" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B18" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B19" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -6990,35 +6953,35 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="22" customFormat="1" ht="15">
+    <row r="1" spans="1:3" s="22" customFormat="1">
       <c r="A1" s="22" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.5">
+      <c r="A3" s="23" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75">
-      <c r="A3" s="23" t="s">
+      <c r="B3" s="23" t="s">
         <v>441</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="C3" s="23" t="s">
         <v>442</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="15">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B5" s="1">
         <v>23</v>
@@ -7027,9 +6990,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B6" s="1">
         <v>20</v>
@@ -7038,9 +7001,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -7049,14 +7012,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15">
+    <row r="8" spans="1:3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="15">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
@@ -7065,9 +7028,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B10" s="1">
         <v>16</v>
@@ -7076,9 +7039,9 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -7087,7 +7050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -7099,72 +7062,72 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F0996A5-6361-409F-A7D0-A30EB8CCF5CC}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView topLeftCell="L27" workbookViewId="0">
       <selection activeCell="T32" sqref="T31:AH32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" customWidth="1"/>
+    <col min="10" max="10" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" ht="15">
+    <row r="1" spans="1:15" s="16" customFormat="1">
       <c r="A1" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>450</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>451</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>452</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>453</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>454</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>455</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>456</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>457</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>458</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>460</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>461</v>
       </c>
       <c r="M1" s="15" t="s">
         <v>373</v>
       </c>
       <c r="N1" s="15" t="s">
+        <v>461</v>
+      </c>
+      <c r="O1" s="15" t="s">
         <v>462</v>
       </c>
-      <c r="O1" s="15" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15">
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -7183,49 +7146,49 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="60.75">
+    <row r="3" spans="1:15" ht="43.5">
       <c r="A3" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="11" t="s">
         <v>467</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>468</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>471</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="13.5" customHeight="1">
@@ -7245,7 +7208,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="15">
+    <row r="5" spans="1:15">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -7262,52 +7225,52 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="76.5">
+    <row r="6" spans="1:15" ht="58">
       <c r="A6" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>477</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>478</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>480</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="K6" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="L6" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15">
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -7324,7 +7287,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="15">
+    <row r="8" spans="1:15">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -7341,52 +7304,52 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="76.5">
+    <row r="9" spans="1:15" ht="72.5">
       <c r="A9" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>485</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>486</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>487</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="J9" s="11" t="s">
         <v>488</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="K9" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="N9" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="O9" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15">
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -7403,7 +7366,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="15">
+    <row r="11" spans="1:15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -7420,52 +7383,52 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="91.5">
+    <row r="12" spans="1:15" ht="87">
       <c r="A12" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>491</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>492</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="J12" s="11" t="s">
         <v>494</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="K12" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15">
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -7482,7 +7445,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="15">
+    <row r="14" spans="1:15">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -7499,52 +7462,52 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="91.5">
+    <row r="15" spans="1:15" ht="87">
       <c r="A15" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>497</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>498</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="J15" s="11" t="s">
         <v>500</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="K15" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="O15" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="15">
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -7561,7 +7524,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="15">
+    <row r="17" spans="1:15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -7578,52 +7541,52 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" ht="91.5">
+    <row r="18" spans="1:15" ht="87">
       <c r="A18" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>505</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>506</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I18" s="11" t="s">
+        <v>506</v>
+      </c>
+      <c r="J18" s="11" t="s">
         <v>507</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="K18" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="15">
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -7640,7 +7603,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" ht="15">
+    <row r="20" spans="1:15">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -7657,52 +7620,52 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" ht="60.75">
+    <row r="21" spans="1:15" ht="43.5">
       <c r="A21" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>510</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>511</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="J21" s="11" t="s">
         <v>513</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="K21" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="15">
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -7719,7 +7682,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:15" ht="15">
+    <row r="23" spans="1:15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -7736,52 +7699,52 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="1:15" ht="91.5">
+    <row r="24" spans="1:15" ht="87">
       <c r="A24" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>516</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>517</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I24" s="11" t="s">
+        <v>517</v>
+      </c>
+      <c r="J24" s="11" t="s">
         <v>518</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="K24" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="O24" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15">
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -7798,7 +7761,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="1:15" ht="15">
+    <row r="26" spans="1:15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -7817,48 +7780,48 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="1:15" ht="60.75">
+    <row r="27" spans="1:15" ht="58">
       <c r="A27" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>521</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>522</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="11" t="s">
         <v>524</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="J27" s="1" t="s">
         <v>525</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>526</v>
-      </c>
       <c r="K27" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:15" ht="15">
+    <row r="28" spans="1:15">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -7875,25 +7838,15 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="1:15" ht="15"/>
-    <row r="30" spans="1:15" ht="15"/>
-    <row r="31" spans="1:15" ht="15"/>
-    <row r="32" spans="1:15" ht="15"/>
-    <row r="33" ht="15"/>
-    <row r="34" ht="15"/>
-    <row r="35" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8094,19 +8047,46 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA60C45-E1DB-4EB3-968D-8F51BAA4D6BE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0F17411-1201-402A-A908-7BB4E026989D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B64156A-488B-40A5-BAE1-9317979EE680}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B64156A-488B-40A5-BAE1-9317979EE680}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f6f59140-29a7-47f4-adbd-055f93383ed7"/>
+    <ds:schemaRef ds:uri="8a4a2c7e-2ccc-49d7-a0a9-0d60de059ae0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0F17411-1201-402A-A908-7BB4E026989D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA60C45-E1DB-4EB3-968D-8F51BAA4D6BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>